<commit_message>
updated buffer address with mail from SEEED
</commit_message>
<xml_diff>
--- a/Modbus_protocol/buffer_addresses.xlsx
+++ b/Modbus_protocol/buffer_addresses.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t xml:space="preserve">Identification (from doc manual)</t>
   </si>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">0x1002</t>
   </si>
   <si>
-    <t xml:space="preserve">probably same value as above</t>
+    <t xml:space="preserve">calculation coeff for calibration factor 1 (mail Seeed)</t>
   </si>
   <si>
     <t xml:space="preserve">ODO slope calibration, calibration in air saturated water</t>
@@ -154,6 +154,9 @@
     <t xml:space="preserve">0x1004</t>
   </si>
   <si>
+    <t xml:space="preserve">calculated coefficient for calibration factor 2 (mail Seeed)</t>
+  </si>
+  <si>
     <t xml:space="preserve">sensor ID number</t>
   </si>
   <si>
@@ -169,13 +172,13 @@
     <t xml:space="preserve">0x0005</t>
   </si>
   <si>
-    <t xml:space="preserve">unknown</t>
+    <t xml:space="preserve">device identification ( mail seeed)</t>
   </si>
   <si>
     <t xml:space="preserve">0x2002</t>
   </si>
   <si>
-    <t xml:space="preserve">suspecte sensor ID gaian</t>
+    <t xml:space="preserve">device address (mail Seeed)</t>
   </si>
   <si>
     <t xml:space="preserve">baud rate</t>
@@ -193,7 +196,7 @@
     <t xml:space="preserve">0x07E8</t>
   </si>
   <si>
-    <t xml:space="preserve">suspected building year</t>
+    <t xml:space="preserve">year of factory shipment (mail Seeed)</t>
   </si>
   <si>
     <t xml:space="preserve">0x2005</t>
@@ -202,7 +205,10 @@
     <t xml:space="preserve">0x0130</t>
   </si>
   <si>
-    <t xml:space="preserve">suspected sensor S/N</t>
+    <t xml:space="preserve">date of factory shipment (mail Seeed) Day month ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resst to factory settings</t>
   </si>
   <si>
     <t xml:space="preserve">w</t>
@@ -340,14 +346,14 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="63.03"/>
@@ -713,16 +719,19 @@
       <c r="H14" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I14" s="0" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>8192</v>
@@ -734,7 +743,7 @@
         <v>55</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>12</v>
@@ -746,7 +755,7 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>8193</v>
@@ -758,13 +767,13 @@
         <v>5</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,7 +782,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>8194</v>
@@ -785,22 +794,22 @@
         <v>55</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>8195</v>
@@ -818,7 +827,7 @@
         <v>12</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,7 +836,7 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>8196</v>
@@ -839,13 +848,13 @@
         <v>2024</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,7 +863,7 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>8197</v>
@@ -866,47 +875,47 @@
         <v>304</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>8224</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated buffer address with addresses not to change
</commit_message>
<xml_diff>
--- a/Modbus_protocol/buffer_addresses.xlsx
+++ b/Modbus_protocol/buffer_addresses.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t xml:space="preserve">Identification (from doc manual)</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t xml:space="preserve">Total addresses that responded Ok to the scanning done with mbpoll software on linux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not change values in addresses in red.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this may cause the device to become damaged or inoperable. (SEEED mail)</t>
   </si>
 </sst>
 </file>
@@ -236,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -258,6 +264,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -309,7 +329,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -326,6 +346,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,6 +367,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -343,13 +435,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.33"/>
@@ -643,25 +735,25 @@
       <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="4" t="n">
         <v>4098</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="4" t="n">
         <v>739</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="4" t="n">
         <v>739</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="0" t="s">
+      <c r="H12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -701,25 +793,25 @@
       <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="4" t="n">
         <v>4100</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="4" t="n">
         <v>2206</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="4" t="n">
         <v>2206</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="0" t="s">
+      <c r="H14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -754,25 +846,25 @@
         <v>36</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="4" t="n">
         <v>8193</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="0" t="s">
+      <c r="H16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -781,25 +873,25 @@
         <v>36</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="4" t="n">
         <v>8194</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="4" t="n">
         <v>55</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="4" t="n">
         <v>55</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="0" t="s">
+      <c r="H17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -835,25 +927,25 @@
         <v>36</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="4" t="n">
         <v>8196</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="4" t="n">
         <v>2024</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="4" t="n">
         <v>2024</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="0" t="s">
+      <c r="H19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -862,25 +954,25 @@
         <v>36</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="4" t="n">
         <v>8197</v>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="4" t="n">
         <v>304</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="4" t="n">
         <v>304</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="0" t="s">
+      <c r="H20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -918,9 +1010,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="0" t="n">
-        <v>8224</v>
+    <row r="26" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>